<commit_message>
Updated values with more steps
</commit_message>
<xml_diff>
--- a/ATXOutputVoltageRailSpecifications.xlsx
+++ b/ATXOutputVoltageRailSpecifications.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\EEE\Year 3\ELEC60024 Power Electronics\coursework\ATX_PowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644EE67D-A457-4C5F-9255-FC31BAF7EEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A50668-B736-423C-ACFF-88E07EFC34B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{6E9D288D-CD69-4052-B821-7AE9FF5B3C3B}"/>
+    <workbookView xWindow="-23420" yWindow="2470" windowWidth="17300" windowHeight="10060" activeTab="1" xr2:uid="{6E9D288D-CD69-4052-B821-7AE9FF5B3C3B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VoltageRailSpec" sheetId="1" r:id="rId1"/>
+    <sheet name="Task4_Efficiency" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Supply (V)</t>
   </si>
@@ -83,6 +84,24 @@
   </si>
   <si>
     <t>Output Pwr (W)</t>
+  </si>
+  <si>
+    <t>$I_{in}$ (A)</t>
+  </si>
+  <si>
+    <t>$V_{out}$ (V)</t>
+  </si>
+  <si>
+    <t>$I_{out}$ (A)</t>
+  </si>
+  <si>
+    <t>Efficiency $\eta$</t>
+  </si>
+  <si>
+    <t>$V_{in}$ (V)</t>
+  </si>
+  <si>
+    <t>$R_{load}$ ($\Omega$)</t>
   </si>
 </sst>
 </file>
@@ -436,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B407FFA1-C9B8-40C6-B120-79A74EF449CA}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -638,4 +657,235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D7509D-6143-42B3-B978-6F626A61E7BB}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F10" sqref="A1:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>92.061400000000006</v>
+      </c>
+      <c r="D2">
+        <v>88.345399999999998</v>
+      </c>
+      <c r="E2">
+        <v>35.767400000000002</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2/C2/B2</f>
+        <v>0.34323671592654464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>12.35</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>61.257800000000003</v>
+      </c>
+      <c r="D3">
+        <v>179.64099999999999</v>
+      </c>
+      <c r="E3">
+        <v>14.5458</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3/C3/B3</f>
+        <v>0.4265615248670373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>24.7</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>44.874400000000001</v>
+      </c>
+      <c r="D4">
+        <v>259.55599999999998</v>
+      </c>
+      <c r="E4">
+        <v>10.5083</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4/C4/B4</f>
+        <v>0.60780585696967526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>123.5</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>13.1896</v>
+      </c>
+      <c r="D5">
+        <v>377.67</v>
+      </c>
+      <c r="E5">
+        <v>3.0580500000000002</v>
+      </c>
+      <c r="F5">
+        <f>D5*E5/C5/B5</f>
+        <v>0.87563970363013299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>11.305899999999999</v>
+      </c>
+      <c r="D6">
+        <v>388.214</v>
+      </c>
+      <c r="E6">
+        <v>2.6195300000000001</v>
+      </c>
+      <c r="F6">
+        <f>D6*E6/C6/B6</f>
+        <v>0.89947568917114085</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>172.9</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>9.8307599999999997</v>
+      </c>
+      <c r="D7">
+        <v>393.375</v>
+      </c>
+      <c r="E7">
+        <v>2.2751600000000001</v>
+      </c>
+      <c r="F7">
+        <f>D7*E7/C7/B7</f>
+        <v>0.91039865178277168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>197.6</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>8.69834</v>
+      </c>
+      <c r="D8">
+        <v>397.339</v>
+      </c>
+      <c r="E8">
+        <v>2.0108199999999998</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F10" si="0">D8*E8/C8/B8</f>
+        <v>0.91853986850364533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>222.3</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>7.8016399999999999</v>
+      </c>
+      <c r="D9">
+        <v>400.47899999999998</v>
+      </c>
+      <c r="E9">
+        <v>1.80152</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.92476828984675019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>247</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>7.0739999999999998</v>
+      </c>
+      <c r="D10">
+        <v>403.02699999999999</v>
+      </c>
+      <c r="E10">
+        <v>1.6316900000000001</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.9296227390867966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Rise and Settling Time Measurements
</commit_message>
<xml_diff>
--- a/ATXOutputVoltageRailSpecifications.xlsx
+++ b/ATXOutputVoltageRailSpecifications.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\EEE\Year 3\ELEC60024 Power Electronics\coursework\ATX_PowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A50668-B736-423C-ACFF-88E07EFC34B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ECD0DB-8843-4C41-9641-E40A704C58FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23420" yWindow="2470" windowWidth="17300" windowHeight="10060" activeTab="1" xr2:uid="{6E9D288D-CD69-4052-B821-7AE9FF5B3C3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{6E9D288D-CD69-4052-B821-7AE9FF5B3C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="VoltageRailSpec" sheetId="1" r:id="rId1"/>
     <sheet name="Task4_Efficiency" sheetId="2" r:id="rId2"/>
+    <sheet name="Task4_StartupBehaviour" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Supply (V)</t>
   </si>
@@ -102,6 +103,48 @@
   </si>
   <si>
     <t>$R_{load}$ ($\Omega$)</t>
+  </si>
+  <si>
+    <t>$V_{out, max}$ (V)</t>
+  </si>
+  <si>
+    <t>Overshoot (%)</t>
+  </si>
+  <si>
+    <t>$\Eta &lt; 0.05 V_{out}$</t>
+  </si>
+  <si>
+    <t>Rise Time (s)</t>
+  </si>
+  <si>
+    <t>Settling Time (s)</t>
+  </si>
+  <si>
+    <t>~~0.0199981~~</t>
+  </si>
+  <si>
+    <t>~~0.0199986~~</t>
+  </si>
+  <si>
+    <t>~~0.0199984~~</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>Rise Time from 0.1 $V_{out}$ to 0.9$V_{out}$</t>
+  </si>
+  <si>
+    <t>~~-0.00133999~~</t>
+  </si>
+  <si>
+    <t>~~0.0046~~</t>
+  </si>
+  <si>
+    <t>~~0.00604003~~</t>
   </si>
 </sst>
 </file>
@@ -137,8 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D7509D-6143-42B3-B978-6F626A61E7BB}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
@@ -713,7 +759,7 @@
         <v>35.767400000000002</v>
       </c>
       <c r="F2">
-        <f>D2*E2/C2/B2</f>
+        <f t="shared" ref="F2:F7" si="0">D2*E2/C2/B2</f>
         <v>0.34323671592654464</v>
       </c>
     </row>
@@ -734,7 +780,7 @@
         <v>14.5458</v>
       </c>
       <c r="F3">
-        <f>D3*E3/C3/B3</f>
+        <f t="shared" si="0"/>
         <v>0.4265615248670373</v>
       </c>
     </row>
@@ -755,7 +801,7 @@
         <v>10.5083</v>
       </c>
       <c r="F4">
-        <f>D4*E4/C4/B4</f>
+        <f t="shared" si="0"/>
         <v>0.60780585696967526</v>
       </c>
     </row>
@@ -776,7 +822,7 @@
         <v>3.0580500000000002</v>
       </c>
       <c r="F5">
-        <f>D5*E5/C5/B5</f>
+        <f t="shared" si="0"/>
         <v>0.87563970363013299</v>
       </c>
     </row>
@@ -797,7 +843,7 @@
         <v>2.6195300000000001</v>
       </c>
       <c r="F6">
-        <f>D6*E6/C6/B6</f>
+        <f t="shared" si="0"/>
         <v>0.89947568917114085</v>
       </c>
     </row>
@@ -818,7 +864,7 @@
         <v>2.2751600000000001</v>
       </c>
       <c r="F7">
-        <f>D7*E7/C7/B7</f>
+        <f t="shared" si="0"/>
         <v>0.91039865178277168</v>
       </c>
     </row>
@@ -839,7 +885,7 @@
         <v>2.0108199999999998</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F10" si="0">D8*E8/C8/B8</f>
+        <f t="shared" ref="F8:F10" si="1">D8*E8/C8/B8</f>
         <v>0.91853986850364533</v>
       </c>
     </row>
@@ -860,7 +906,7 @@
         <v>1.80152</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.92476828984675019</v>
       </c>
     </row>
@@ -881,8 +927,310 @@
         <v>1.6316900000000001</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9296227390867966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D5A86-60FA-4F48-9FDC-D6A29FDF3E65}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="B3">
+        <v>88.345399999999998</v>
+      </c>
+      <c r="C3">
+        <v>158.83600000000001</v>
+      </c>
+      <c r="D3">
+        <f>(C3-B3)/B3</f>
+        <v>0.79789779660287929</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>4.0901699999999997E-3</v>
+      </c>
+      <c r="G3">
+        <v>2.7501700000000001E-3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>12.35</v>
+      </c>
+      <c r="B4">
+        <v>179.64099999999999</v>
+      </c>
+      <c r="C4">
+        <v>233.45500000000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D11" si="0">(C4-B4)/B4</f>
+        <v>0.29956413068286208</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4">
+        <v>3.4102500000000001E-3</v>
+      </c>
+      <c r="G4">
+        <v>8.01025E-3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>24.7</v>
+      </c>
+      <c r="B5">
+        <v>259.55599999999998</v>
+      </c>
+      <c r="C5">
+        <v>297.37</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.14568725053553</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>2.1101599999999998E-3</v>
+      </c>
+      <c r="G5">
+        <v>8.1501799999999999E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>123.5</v>
+      </c>
+      <c r="B6">
+        <v>377.67</v>
+      </c>
+      <c r="C6">
+        <v>387.16800000000001</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.5148939550401119E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.6602000000000002E-3</v>
+      </c>
+      <c r="F6">
+        <v>6.4998699999999998E-4</v>
+      </c>
+      <c r="G6">
+        <v>3.3101900000000002E-3</v>
+      </c>
+      <c r="H6">
+        <v>5.1478499999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="B7">
+        <v>388.214</v>
+      </c>
+      <c r="C7">
+        <v>397.96800000000002</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2.5125317479534531E-2</v>
+      </c>
+      <c r="E7">
+        <v>2.2806900000000001E-3</v>
+      </c>
+      <c r="F7">
+        <v>5.9952699999999998E-4</v>
+      </c>
+      <c r="G7">
+        <v>2.8802200000000002E-3</v>
+      </c>
+      <c r="H7">
+        <v>4.1478599999999997E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>172.9</v>
+      </c>
+      <c r="B8">
+        <v>393.375</v>
+      </c>
+      <c r="C8">
+        <v>402.20699999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2.2451858913250699E-2</v>
+      </c>
+      <c r="E8">
+        <v>1.9201000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>5.4996799999999996E-4</v>
+      </c>
+      <c r="G8">
+        <v>2.47007E-3</v>
+      </c>
+      <c r="H8">
+        <v>3.4278999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>197.6</v>
+      </c>
+      <c r="B9">
+        <v>397.339</v>
+      </c>
+      <c r="C9">
+        <v>405.423</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2.0345347423736414E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.6203000000000001E-3</v>
+      </c>
+      <c r="F9">
+        <v>5.1978699999999996E-4</v>
+      </c>
+      <c r="G9">
+        <v>2.1400799999999999E-3</v>
+      </c>
+      <c r="H9">
+        <v>2.8179099999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>222.3</v>
+      </c>
+      <c r="B10">
+        <v>400.47899999999998</v>
+      </c>
+      <c r="C10">
+        <v>407.952</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.8660154465028164E-2</v>
+      </c>
+      <c r="E10">
+        <v>1.39993E-3</v>
+      </c>
+      <c r="F10">
+        <v>4.9010099999999995E-4</v>
+      </c>
+      <c r="G10">
+        <v>1.89003E-3</v>
+      </c>
+      <c r="H10">
+        <v>2.3479299999999998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>247</v>
+      </c>
+      <c r="B11">
+        <v>403.02699999999999</v>
+      </c>
+      <c r="C11">
+        <v>409.983</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.7259389569433358E-2</v>
+      </c>
+      <c r="E11">
+        <v>1.2301899999999999E-3</v>
+      </c>
+      <c r="F11">
+        <v>4.6982099999999999E-4</v>
+      </c>
+      <c r="G11">
+        <v>1.7000100000000001E-3</v>
+      </c>
+      <c r="H11">
+        <v>2.00796E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inductor core selected (Damn you Magnetics)
</commit_message>
<xml_diff>
--- a/ATXOutputVoltageRailSpecifications.xlsx
+++ b/ATXOutputVoltageRailSpecifications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\EEE\Year 3\ELEC60024 Power Electronics\coursework\ATX_PowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019D6FD2-ABAC-479C-A1B5-A207E60EA966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203FB68D-6A4F-4331-BCB7-068BBD11830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="4" activeTab="9" xr2:uid="{6E9D288D-CD69-4052-B821-7AE9FF5B3C3B}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13763" uniqueCount="2711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13781" uniqueCount="2722">
   <si>
     <t>Supply (V)</t>
   </si>
@@ -8197,13 +8197,46 @@
     <t>MPP, Kool Mu Max have lower losses compared to Kool Mu, High mu have lower losses compared to Xflux</t>
   </si>
   <si>
-    <t>Core loss</t>
-  </si>
-  <si>
-    <t>Temperature Rise</t>
-  </si>
-  <si>
     <t>6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required Ripple </t>
+  </si>
+  <si>
+    <t>Method 1</t>
+  </si>
+  <si>
+    <t>H,Acmin</t>
+  </si>
+  <si>
+    <t>H,Acmax</t>
+  </si>
+  <si>
+    <t>Flux Density B, Max</t>
+  </si>
+  <si>
+    <t>Flux Density B, Min</t>
+  </si>
+  <si>
+    <t>Using Spreadsheet</t>
+  </si>
+  <si>
+    <t>Bpeak</t>
+  </si>
+  <si>
+    <t>Power Loss (mW/cc)</t>
+  </si>
+  <si>
+    <t>Core loss (mW)</t>
+  </si>
+  <si>
+    <t>Loss limited not bias (current) limited anymore</t>
+  </si>
+  <si>
+    <t>Total losses/Surface Area</t>
+  </si>
+  <si>
+    <t>Temperature Rise (degrees celscius)</t>
   </si>
 </sst>
 </file>
@@ -8884,12 +8917,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC9CD1E-468A-4075-9014-DECE2A3DC0DE}">
-  <dimension ref="A1:AC29"/>
+  <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="X1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="AC12" sqref="AC12"/>
+      <selection pane="topRight" activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8912,14 +8945,15 @@
     <col min="19" max="19" width="10.5546875" customWidth="1"/>
     <col min="21" max="21" width="11.5546875" customWidth="1"/>
     <col min="26" max="26" width="10.5546875" customWidth="1"/>
+    <col min="35" max="35" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2691</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2694</v>
       </c>
@@ -8927,7 +8961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2695</v>
       </c>
@@ -8938,7 +8972,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2696</v>
       </c>
@@ -8946,7 +8980,7 @@
         <v>8.26</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2697</v>
       </c>
@@ -8954,7 +8988,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2703</v>
       </c>
@@ -8962,21 +8996,21 @@
         <v>1.044E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2640</v>
       </c>
       <c r="B8" s="17">
         <v>2.6199999999999999E-3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="24" t="s">
         <v>2642</v>
       </c>
       <c r="D8" t="s">
         <v>2645</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2641</v>
       </c>
@@ -8987,937 +9021,1091 @@
         <v>2672</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>2709</v>
+      </c>
+      <c r="B10">
+        <v>0.57150000000000001</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>2719</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>2634</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>2635</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q12" t="s">
         <v>2687</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U12" t="s">
         <v>2690</v>
       </c>
+      <c r="AB12" t="s">
+        <v>2710</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>2715</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>2715</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>2720</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>2679</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F13" t="s">
         <v>2680</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G13" t="s">
         <v>2680</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H13" t="s">
         <v>2680</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I13" t="s">
         <v>2680</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J13" t="s">
         <v>2680</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K13" t="s">
         <v>2680</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L13" t="s">
         <v>2680</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M13" t="s">
         <v>2680</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N13" t="s">
         <v>2681</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O13" t="s">
         <v>2682</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P13" t="s">
         <v>2683</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q13" t="s">
         <v>2684</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R13" t="s">
         <v>2681</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S13" t="s">
         <v>2682</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T13" t="s">
         <v>2683</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U13" t="s">
         <v>2683</v>
       </c>
-      <c r="V11">
+      <c r="V13">
         <v>5</v>
       </c>
-      <c r="W11">
+      <c r="W13">
         <v>5</v>
       </c>
-      <c r="X11" t="s">
+      <c r="X13" t="s">
         <v>2692</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y13" t="s">
         <v>2692</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Z13" t="s">
         <v>2701</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA13" t="s">
         <v>2701</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB13" t="s">
         <v>2705</v>
       </c>
-      <c r="AC11" t="s">
-        <v>2710</v>
+      <c r="AC13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>2705</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>2708</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="14" spans="1:35" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>2636</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>2637</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" t="s">
         <v>2654</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>2666</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>2624</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>2667</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>2668</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>2669</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>2670</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>2673</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>2639</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>2675</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>2674</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>2676</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>2677</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>2678</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>2685</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>2686</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>2688</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U14" s="1" t="s">
         <v>2689</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>2693</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>2698</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>2700</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>2699</v>
       </c>
-      <c r="Z12" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>2702</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AA14" s="1" t="s">
         <v>2704</v>
       </c>
-      <c r="AB12" s="1" t="s">
-        <v>2708</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>2709</v>
+      <c r="AB14" s="1" t="s">
+        <v>2712</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>2711</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>2713</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>2714</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>2716</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>2717</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>2718</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>2721</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>2648</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>77868</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>123</v>
       </c>
-      <c r="E13">
+      <c r="E15" s="5">
         <v>77.8</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>12.7</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>176</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>196</v>
-      </c>
-      <c r="I13">
-        <f>G13*H13</f>
-        <v>34496</v>
-      </c>
-      <c r="J13">
-        <v>26</v>
-      </c>
-      <c r="K13">
-        <v>30</v>
-      </c>
-      <c r="L13">
-        <f>K13*0.92</f>
-        <v>27.6</v>
-      </c>
-      <c r="M13">
-        <f>SQRT($B$8*(10^6)*(10^3)/L13)</f>
-        <v>308.10312596902367</v>
-      </c>
-      <c r="N13">
-        <f>4*PI()*M13*$B$9/H13</f>
-        <v>150.52369429068563</v>
-      </c>
-      <c r="O13">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="P13" s="17">
-        <f>$B$8*O13</f>
-        <v>1.7685000000000001E-3</v>
-      </c>
-      <c r="Q13">
-        <f>M13/O13</f>
-        <v>456.44907550966468</v>
-      </c>
-      <c r="R13">
-        <f>4*PI()*Q13*$B$9/H13</f>
-        <v>222.99806561583054</v>
-      </c>
-      <c r="S13">
-        <v>0.5</v>
-      </c>
-      <c r="T13">
-        <f>K13*S13</f>
-        <v>15</v>
-      </c>
-      <c r="U13">
-        <f>T13*Q13^2/1000</f>
-        <v>3125.1863780044137</v>
-      </c>
-      <c r="V13">
-        <f>$B$3*Q13</f>
-        <v>8.3986629893778293</v>
-      </c>
-      <c r="W13">
-        <f>V13*10^2</f>
-        <v>839.86629893778297</v>
-      </c>
-      <c r="X13">
-        <v>1820</v>
-      </c>
-      <c r="Y13">
-        <f>W13/X13</f>
-        <v>0.46146499941636426</v>
-      </c>
-      <c r="Z13">
-        <f>W13/(1000)*$B$6</f>
-        <v>8.7682041609104533E-3</v>
-      </c>
-      <c r="AA13">
-        <f>$B$9^2*Z13</f>
-        <v>0.50912051368076894</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>2648</v>
-      </c>
-      <c r="B14">
-        <v>77908</v>
-      </c>
-      <c r="C14">
-        <v>124</v>
-      </c>
-      <c r="E14">
-        <v>77.8</v>
-      </c>
-      <c r="F14">
-        <v>15.88</v>
-      </c>
-      <c r="G14">
-        <v>221</v>
-      </c>
-      <c r="H14">
-        <v>196</v>
-      </c>
-      <c r="I14">
-        <f>G14*H14</f>
-        <v>43316</v>
-      </c>
-      <c r="J14">
-        <v>26</v>
-      </c>
-      <c r="K14">
-        <v>37</v>
-      </c>
-      <c r="L14">
-        <f t="shared" ref="L14:L20" si="0">K14*0.92</f>
-        <v>34.04</v>
-      </c>
-      <c r="M14">
-        <f>SQRT($B$8*(10^6)*(10^3)/L14)</f>
-        <v>277.43156385034223</v>
-      </c>
-      <c r="N14">
-        <f>4*PI()*M14*$B$9/H14</f>
-        <v>135.53911136816652</v>
-      </c>
-      <c r="O14">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="P14" s="17">
-        <f>$B$8*O14</f>
-        <v>1.8732999999999998E-3</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" ref="Q14:Q20" si="1">M14/O14</f>
-        <v>388.01617321726189</v>
-      </c>
-      <c r="R14">
-        <f>4*PI()*Q14*$B$9/H14</f>
-        <v>189.56519072470846</v>
-      </c>
-      <c r="S14">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="T14">
-        <f t="shared" ref="T14:T20" si="2">K14*S14</f>
-        <v>21.274999999999999</v>
-      </c>
-      <c r="U14">
-        <f t="shared" ref="U14:U20" si="3">T14*Q14^2/1000</f>
-        <v>3203.0906156780284</v>
-      </c>
-      <c r="V14">
-        <f t="shared" ref="V14:V20" si="4">$B$3*Q14</f>
-        <v>7.139497587197619</v>
-      </c>
-      <c r="W14">
-        <f t="shared" ref="W14:W20" si="5">V14*10^2</f>
-        <v>713.94975871976192</v>
-      </c>
-      <c r="X14">
-        <v>1820</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" ref="Y14:Y20" si="6">W14/X14</f>
-        <v>0.39228008720866037</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" ref="Z14:Z20" si="7">W14/(1000)*$B$6</f>
-        <v>7.4536354810343149E-3</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" ref="AA14:AA20" si="8">$B$9^2*Z14</f>
-        <v>0.43279087202496885</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
-        <v>2649</v>
-      </c>
-      <c r="B15">
-        <v>79617</v>
-      </c>
-      <c r="C15">
-        <v>120</v>
-      </c>
-      <c r="E15">
-        <v>62</v>
-      </c>
-      <c r="F15">
-        <v>24.99</v>
-      </c>
-      <c r="G15">
-        <v>360</v>
-      </c>
-      <c r="H15">
-        <v>144</v>
       </c>
       <c r="I15">
         <f>G15*H15</f>
+        <v>34496</v>
+      </c>
+      <c r="J15">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>30</v>
+      </c>
+      <c r="L15">
+        <f>K15*0.92</f>
+        <v>27.6</v>
+      </c>
+      <c r="M15">
+        <f>SQRT($B$8*(10^6)*(10^3)/L15)</f>
+        <v>308.10312596902367</v>
+      </c>
+      <c r="N15">
+        <f>4*PI()*M15*$B$9/H15</f>
+        <v>150.52369429068563</v>
+      </c>
+      <c r="O15">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="P15" s="17">
+        <f>$B$8*O15</f>
+        <v>1.7685000000000001E-3</v>
+      </c>
+      <c r="Q15">
+        <f>M15/O15</f>
+        <v>456.44907550966468</v>
+      </c>
+      <c r="R15">
+        <f>4*PI()*Q15*$B$9/H15</f>
+        <v>222.99806561583054</v>
+      </c>
+      <c r="S15">
+        <v>0.5</v>
+      </c>
+      <c r="T15">
+        <f>K15*S15</f>
+        <v>15</v>
+      </c>
+      <c r="U15">
+        <f>T15*Q15^2/1000</f>
+        <v>3125.1863780044137</v>
+      </c>
+      <c r="V15">
+        <f>$B$3*Q15</f>
+        <v>8.3986629893778293</v>
+      </c>
+      <c r="W15">
+        <f>V15*10^2</f>
+        <v>839.86629893778297</v>
+      </c>
+      <c r="X15">
+        <v>1820</v>
+      </c>
+      <c r="Y15" s="5">
+        <f>W15/X15</f>
+        <v>0.46146499941636426</v>
+      </c>
+      <c r="Z15">
+        <f>W15/(1000)*$B$6</f>
+        <v>8.7682041609104533E-3</v>
+      </c>
+      <c r="AA15">
+        <f>$B$9^2*Z15</f>
+        <v>0.50912051368076894</v>
+      </c>
+      <c r="AB15">
+        <f>4*PI()*Q15/H15*($B$9+$B$10/2)</f>
+        <v>231.36049307642418</v>
+      </c>
+      <c r="AC15">
+        <f>4*PI()*Q15/H15*($B$9-$B$10/2)</f>
+        <v>214.63563815523688</v>
+      </c>
+      <c r="AD15">
+        <v>0.4592</v>
+      </c>
+      <c r="AE15">
+        <v>0.43740000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>2648</v>
+      </c>
+      <c r="B16">
+        <v>77908</v>
+      </c>
+      <c r="C16">
+        <v>124</v>
+      </c>
+      <c r="E16" s="5">
+        <v>77.8</v>
+      </c>
+      <c r="F16">
+        <v>15.88</v>
+      </c>
+      <c r="G16">
+        <v>221</v>
+      </c>
+      <c r="H16">
+        <v>196</v>
+      </c>
+      <c r="I16">
+        <f>G16*H16</f>
+        <v>43316</v>
+      </c>
+      <c r="J16">
+        <v>26</v>
+      </c>
+      <c r="K16">
+        <v>37</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L22" si="0">K16*0.92</f>
+        <v>34.04</v>
+      </c>
+      <c r="M16">
+        <f>SQRT($B$8*(10^6)*(10^3)/L16)</f>
+        <v>277.43156385034223</v>
+      </c>
+      <c r="N16">
+        <f>4*PI()*M16*$B$9/H16</f>
+        <v>135.53911136816652</v>
+      </c>
+      <c r="O16">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="P16" s="17">
+        <f>$B$8*O16</f>
+        <v>1.8732999999999998E-3</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ref="Q16:Q22" si="1">M16/O16</f>
+        <v>388.01617321726189</v>
+      </c>
+      <c r="R16">
+        <f>4*PI()*Q16*$B$9/H16</f>
+        <v>189.56519072470846</v>
+      </c>
+      <c r="S16">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="T16">
+        <f t="shared" ref="T16:T22" si="2">K16*S16</f>
+        <v>21.274999999999999</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ref="U16:U22" si="3">T16*Q16^2/1000</f>
+        <v>3203.0906156780284</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ref="V16:V22" si="4">$B$3*Q16</f>
+        <v>7.139497587197619</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ref="W16:W22" si="5">V16*10^2</f>
+        <v>713.94975871976192</v>
+      </c>
+      <c r="X16">
+        <v>1820</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ref="Y16:Y22" si="6">W16/X16</f>
+        <v>0.39228008720866037</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ref="Z16:Z22" si="7">W16/(1000)*$B$6</f>
+        <v>7.4536354810343149E-3</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ref="AA16:AA22" si="8">$B$9^2*Z16</f>
+        <v>0.43279087202496885</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" ref="AB16:AB22" si="9">4*PI()*Q16/H16*($B$9+$B$10/2)</f>
+        <v>196.67388537688504</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" ref="AC16:AC22" si="10">4*PI()*Q16/H16*($B$9-$B$10/2)</f>
+        <v>182.45649607253191</v>
+      </c>
+      <c r="AD16">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="AE16">
+        <v>0.39140000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>2649</v>
+      </c>
+      <c r="B17">
+        <v>79617</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <v>62</v>
+      </c>
+      <c r="F17">
+        <v>24.99</v>
+      </c>
+      <c r="G17">
+        <v>360</v>
+      </c>
+      <c r="H17">
+        <v>144</v>
+      </c>
+      <c r="I17">
+        <f>G17*H17</f>
         <v>51840</v>
       </c>
-      <c r="J15">
+      <c r="J17">
         <v>60</v>
       </c>
-      <c r="K15">
+      <c r="K17">
         <v>189</v>
       </c>
-      <c r="L15">
+      <c r="L17">
         <f t="shared" si="0"/>
         <v>173.88</v>
       </c>
-      <c r="M15">
-        <f>SQRT($B$8*(10^6)*(10^3)/L15)</f>
+      <c r="M17">
+        <f>SQRT($B$8*(10^6)*(10^3)/L17)</f>
         <v>122.75122359451188</v>
       </c>
-      <c r="N15">
-        <f>4*PI()*M15*$B$9/H15</f>
+      <c r="N17">
+        <f>4*PI()*M17*$B$9/H17</f>
         <v>81.625935779144882</v>
       </c>
-      <c r="O15">
+      <c r="O17">
         <v>0.71699999999999997</v>
       </c>
-      <c r="P15" s="17">
-        <f>$B$8*O15</f>
+      <c r="P17" s="17">
+        <f>$B$8*O17</f>
         <v>1.8785399999999999E-3</v>
       </c>
-      <c r="Q15">
+      <c r="Q17">
         <f t="shared" si="1"/>
         <v>171.20114866738061</v>
       </c>
-      <c r="R15">
-        <f>4*PI()*Q15*$B$9/H15</f>
+      <c r="R17">
+        <f>4*PI()*Q17*$B$9/H17</f>
         <v>113.84370401554378</v>
       </c>
-      <c r="S15">
+      <c r="S17">
         <v>0.56599999999999995</v>
       </c>
-      <c r="T15">
+      <c r="T17">
         <f t="shared" si="2"/>
         <v>106.97399999999999</v>
       </c>
-      <c r="U15">
+      <c r="U17">
         <f t="shared" si="3"/>
         <v>3135.3901079723382</v>
       </c>
-      <c r="V15">
+      <c r="V17">
         <f t="shared" si="4"/>
         <v>3.1501011354798032</v>
       </c>
-      <c r="W15">
+      <c r="W17">
         <f t="shared" si="5"/>
         <v>315.01011354798032</v>
       </c>
-      <c r="X15">
+      <c r="X17">
         <v>789</v>
       </c>
-      <c r="Y15">
+      <c r="Y17">
         <f t="shared" si="6"/>
         <v>0.39925236191125518</v>
       </c>
-      <c r="Z15">
+      <c r="Z17">
         <f t="shared" si="7"/>
         <v>3.2887055854409143E-3</v>
       </c>
-      <c r="AA15">
+      <c r="AA17">
         <f t="shared" si="8"/>
         <v>0.19095671659527541</v>
       </c>
+      <c r="AB17">
+        <f t="shared" si="9"/>
+        <v>118.11284291612668</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="10"/>
+        <v>109.57456511496089</v>
+      </c>
+      <c r="AD17">
+        <v>0.57289999999999996</v>
+      </c>
+      <c r="AE17">
+        <v>0.54430000000000001</v>
+      </c>
+      <c r="AF17">
+        <f t="shared" ref="AF16:AF20" si="11">(AD17-AE17)/2</f>
+        <v>1.4299999999999979E-2</v>
+      </c>
+      <c r="AG17">
+        <v>3.76</v>
+      </c>
+      <c r="AH17" s="29">
+        <f>AG17*G17*H17/1000</f>
+        <v>194.91839999999999</v>
+      </c>
+      <c r="AI17">
+        <f>(AH17+AA17*1000)/G17</f>
+        <v>1.071875323875765</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>2652</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>2651</v>
       </c>
-      <c r="P16" s="17"/>
+      <c r="P18" s="17"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>2650</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <v>78072</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <v>121</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>2655</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>68</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>19.989999999999998</v>
       </c>
-      <c r="G17">
+      <c r="G19">
         <v>314</v>
       </c>
-      <c r="H17">
+      <c r="H19">
         <v>158</v>
       </c>
-      <c r="I17">
-        <f>G17*H17</f>
+      <c r="I19">
+        <f>G19*H19</f>
         <v>49612</v>
       </c>
-      <c r="J17">
+      <c r="J19">
         <v>60</v>
       </c>
-      <c r="K17">
+      <c r="K19">
         <v>143</v>
       </c>
-      <c r="L17">
+      <c r="L19">
         <f t="shared" si="0"/>
         <v>131.56</v>
       </c>
-      <c r="M17">
-        <f>SQRT($B$8*(10^6)*(10^3)/L17)</f>
+      <c r="M19">
+        <f>SQRT($B$8*(10^6)*(10^3)/L19)</f>
         <v>141.12004726811389</v>
       </c>
-      <c r="N17">
-        <f>4*PI()*M17*$B$9/H17</f>
+      <c r="N19">
+        <f>4*PI()*M19*$B$9/H19</f>
         <v>85.525665385841577</v>
       </c>
-      <c r="O17">
+      <c r="O19">
         <v>0.85799999999999998</v>
       </c>
-      <c r="P17" s="17">
-        <f>$B$8*O17</f>
+      <c r="P19" s="17">
+        <f>$B$8*O19</f>
         <v>2.2479599999999998E-3</v>
       </c>
-      <c r="Q17">
+      <c r="Q19">
         <f t="shared" si="1"/>
         <v>164.47557956656632</v>
       </c>
-      <c r="R17">
-        <f>4*PI()*Q17*$B$9/H17</f>
+      <c r="R19">
+        <f>4*PI()*Q19*$B$9/H19</f>
         <v>99.680262687461038</v>
       </c>
-      <c r="S17">
+      <c r="S19">
         <v>0.80100000000000005</v>
       </c>
-      <c r="T17">
+      <c r="T19">
         <f t="shared" si="2"/>
         <v>114.54300000000001</v>
       </c>
-      <c r="U17">
+      <c r="U19">
         <f t="shared" si="3"/>
         <v>3098.6420086450503</v>
       </c>
-      <c r="V17">
+      <c r="V19">
         <f t="shared" si="4"/>
         <v>3.0263506640248203</v>
       </c>
-      <c r="W17">
+      <c r="W19">
         <f t="shared" si="5"/>
         <v>302.63506640248204</v>
       </c>
-      <c r="X17">
+      <c r="X19">
         <v>945</v>
       </c>
-      <c r="Y17">
+      <c r="Y19">
         <f t="shared" si="6"/>
         <v>0.32024874751585403</v>
       </c>
-      <c r="Z17">
+      <c r="Z19">
         <f t="shared" si="7"/>
         <v>3.1595100932419124E-3</v>
       </c>
-      <c r="AA17">
+      <c r="AA19">
         <f t="shared" si="8"/>
         <v>0.1834550578580357</v>
       </c>
+      <c r="AB19">
+        <f t="shared" si="9"/>
+        <v>103.41827253824084</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="10"/>
+        <v>95.942252836681263</v>
+      </c>
+      <c r="AD19">
+        <v>0.58120000000000005</v>
+      </c>
+      <c r="AE19">
+        <v>0.54559999999999997</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="11"/>
+        <v>1.7800000000000038E-2</v>
+      </c>
+      <c r="AG19">
+        <v>17.29</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" ref="AH18:AH20" si="12">AG19*G19*H19/1000</f>
+        <v>857.79147999999986</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" ref="AI18:AI20" si="13">(AH19+AA19*1000)/G19</f>
+        <v>3.3160717766179473</v>
+      </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
         <v>2653</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>58617</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>120</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>2655</v>
       </c>
-      <c r="E18">
-        <v>62</v>
-      </c>
-      <c r="F18">
+      <c r="E20">
+        <v>62</v>
+      </c>
+      <c r="F20">
         <v>24.99</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>360</v>
       </c>
-      <c r="H18">
+      <c r="H20">
         <v>144</v>
       </c>
-      <c r="I18">
-        <f>G18*H18</f>
+      <c r="I20">
+        <f>G20*H20</f>
         <v>51840</v>
       </c>
-      <c r="J18">
+      <c r="J20">
         <v>60</v>
       </c>
-      <c r="K18">
+      <c r="K20">
         <v>189</v>
       </c>
-      <c r="L18">
+      <c r="L20">
         <f t="shared" si="0"/>
         <v>173.88</v>
       </c>
-      <c r="M18">
-        <f>SQRT($B$8*(10^6)*(10^3)/L18)</f>
+      <c r="M20">
+        <f>SQRT($B$8*(10^6)*(10^3)/L20)</f>
         <v>122.75122359451188</v>
       </c>
-      <c r="N18">
-        <f>4*PI()*M18*$B$9/H18</f>
+      <c r="N20">
+        <f>4*PI()*M20*$B$9/H20</f>
         <v>81.625935779144882</v>
       </c>
-      <c r="O18">
+      <c r="O20">
         <v>0.82099999999999995</v>
       </c>
-      <c r="P18" s="17">
-        <f>$B$8*O18</f>
+      <c r="P20" s="17">
+        <f>$B$8*O20</f>
         <v>2.15102E-3</v>
       </c>
-      <c r="Q18">
+      <c r="Q20">
         <f t="shared" si="1"/>
         <v>149.51427965226785</v>
       </c>
-      <c r="R18">
-        <f>4*PI()*Q18*$B$9/H18</f>
+      <c r="R20">
+        <f>4*PI()*Q20*$B$9/H20</f>
         <v>99.42257707569415</v>
       </c>
-      <c r="S18">
+      <c r="S20">
         <v>0.80600000000000005</v>
       </c>
-      <c r="T18">
+      <c r="T20">
         <f t="shared" si="2"/>
         <v>152.334</v>
       </c>
-      <c r="U18">
+      <c r="U20">
         <f t="shared" si="3"/>
         <v>3405.3534222502153</v>
       </c>
-      <c r="V18">
+      <c r="V20">
         <f t="shared" si="4"/>
         <v>2.7510627456017285</v>
       </c>
-      <c r="W18">
+      <c r="W20">
         <f t="shared" si="5"/>
         <v>275.10627456017284</v>
       </c>
-      <c r="X18">
+      <c r="X20">
         <v>789</v>
       </c>
-      <c r="Y18">
+      <c r="Y20">
         <f t="shared" si="6"/>
         <v>0.34867715406866012</v>
       </c>
-      <c r="Z18">
+      <c r="Z20">
         <f t="shared" si="7"/>
         <v>2.8721095064082043E-3</v>
       </c>
-      <c r="AA18">
+      <c r="AA20">
         <f t="shared" si="8"/>
         <v>0.16676731522388855</v>
       </c>
+      <c r="AB20">
+        <f t="shared" si="9"/>
+        <v>103.15092371603268</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="10"/>
+        <v>95.694230435355621</v>
+      </c>
+      <c r="AD20">
+        <v>0.57930000000000004</v>
+      </c>
+      <c r="AE20">
+        <v>0.54430000000000001</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="11"/>
+        <v>1.7500000000000016E-2</v>
+      </c>
+      <c r="AG20">
+        <v>5.28</v>
+      </c>
+      <c r="AH20" s="29">
+        <f t="shared" si="12"/>
+        <v>273.71520000000004</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="13"/>
+        <v>1.2235625422885794</v>
+      </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>2638</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <v>55617</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>120</v>
       </c>
-      <c r="E19">
-        <v>62</v>
-      </c>
-      <c r="F19">
+      <c r="E21">
+        <v>62</v>
+      </c>
+      <c r="F21">
         <v>24.99</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>360</v>
       </c>
-      <c r="H19">
+      <c r="H21">
         <v>144</v>
       </c>
-      <c r="I19">
-        <f>G19*H19</f>
+      <c r="I21">
+        <f>G21*H21</f>
         <v>51840</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>60</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>189</v>
       </c>
-      <c r="L19">
+      <c r="L21">
         <f t="shared" si="0"/>
         <v>173.88</v>
       </c>
-      <c r="M19">
-        <f>SQRT($B$8*(10^6)*(10^3)/L19)</f>
+      <c r="M21">
+        <f>SQRT($B$8*(10^6)*(10^3)/L21)</f>
         <v>122.75122359451188</v>
       </c>
-      <c r="N19">
-        <f>4*PI()*M19*$B$9/H19</f>
+      <c r="N21">
+        <f>4*PI()*M21*$B$9/H21</f>
         <v>81.625935779144882</v>
       </c>
-      <c r="O19">
+      <c r="O21">
         <v>0.65400000000000003</v>
       </c>
-      <c r="P19" s="17">
-        <f>$B$8*O19</f>
+      <c r="P21" s="17">
+        <f>$B$8*O21</f>
         <v>1.7134800000000001E-3</v>
       </c>
-      <c r="Q19">
+      <c r="Q21">
         <f t="shared" si="1"/>
         <v>187.69300243809155</v>
       </c>
-      <c r="R19">
-        <f>4*PI()*Q19*$B$9/H19</f>
+      <c r="R21">
+        <f>4*PI()*Q21*$B$9/H21</f>
         <v>124.81029935649063</v>
       </c>
-      <c r="S19">
+      <c r="S21">
         <v>0.40200000000000002</v>
       </c>
-      <c r="T19">
+      <c r="T21">
         <f t="shared" si="2"/>
         <v>75.978000000000009</v>
       </c>
-      <c r="U19">
+      <c r="U21">
         <f t="shared" si="3"/>
         <v>2676.6033698915212</v>
       </c>
-      <c r="V19">
+      <c r="V21">
         <f t="shared" si="4"/>
         <v>3.4535512448608845</v>
       </c>
-      <c r="W19">
+      <c r="W21">
         <f t="shared" si="5"/>
         <v>345.35512448608847</v>
       </c>
-      <c r="X19">
+      <c r="X21">
         <v>789</v>
       </c>
-      <c r="Y19">
+      <c r="Y21" s="5">
         <f t="shared" si="6"/>
         <v>0.43771245182013746</v>
       </c>
-      <c r="Z19">
+      <c r="Z21">
         <f t="shared" si="7"/>
         <v>3.6055074996347632E-3</v>
       </c>
-      <c r="AA19">
+      <c r="AA21">
         <f t="shared" si="8"/>
         <v>0.20935162966179274</v>
       </c>
+      <c r="AB21">
+        <f t="shared" si="9"/>
+        <v>129.49068558235902</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="10"/>
+        <v>120.12991313062223</v>
+      </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>2638</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>55868</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>123</v>
       </c>
-      <c r="E20">
+      <c r="E22" s="5">
         <v>77.8</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>12.7</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>176</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>196</v>
       </c>
-      <c r="I20">
-        <f>G20*H20</f>
+      <c r="I22">
+        <f>G22*H22</f>
         <v>34496</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>26</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <v>30</v>
       </c>
-      <c r="L20">
+      <c r="L22">
         <f t="shared" si="0"/>
         <v>27.6</v>
       </c>
-      <c r="M20">
-        <f>SQRT($B$8*(10^6)*(10^3)/L20)</f>
+      <c r="M22">
+        <f>SQRT($B$8*(10^6)*(10^3)/L22)</f>
         <v>308.10312596902367</v>
       </c>
-      <c r="N20">
-        <f>4*PI()*M20*$B$9/H20</f>
+      <c r="N22">
+        <f>4*PI()*M22*$B$9/H22</f>
         <v>150.52369429068563</v>
       </c>
-      <c r="O20">
+      <c r="O22">
         <v>0.76300000000000001</v>
       </c>
-      <c r="P20" s="17">
-        <f>$B$8*O20</f>
+      <c r="P22" s="17">
+        <f>$B$8*O22</f>
         <v>1.99906E-3</v>
       </c>
-      <c r="Q20">
+      <c r="Q22">
         <f t="shared" si="1"/>
         <v>403.80488331457883</v>
       </c>
-      <c r="R20">
-        <f>4*PI()*Q20*$B$9/H20</f>
+      <c r="R22">
+        <f>4*PI()*Q22*$B$9/H22</f>
         <v>197.27876053825116</v>
       </c>
-      <c r="S20">
+      <c r="S22">
         <v>0.62</v>
       </c>
-      <c r="T20">
+      <c r="T22">
         <f t="shared" si="2"/>
         <v>18.600000000000001</v>
       </c>
-      <c r="U20">
+      <c r="U22">
         <f t="shared" si="3"/>
         <v>3032.8859384698317</v>
       </c>
-      <c r="V20">
+      <c r="V22">
         <f t="shared" si="4"/>
         <v>7.4300098529882508</v>
       </c>
-      <c r="W20">
+      <c r="W22">
         <f t="shared" si="5"/>
         <v>743.00098529882507</v>
       </c>
-      <c r="X20">
+      <c r="X22">
         <v>1820</v>
       </c>
-      <c r="Y20">
+      <c r="Y22">
         <f t="shared" si="6"/>
         <v>0.40824229961473907</v>
       </c>
-      <c r="Z20">
+      <c r="Z22">
         <f t="shared" si="7"/>
         <v>7.7569302865197337E-3</v>
       </c>
-      <c r="AA20">
+      <c r="AA22">
         <f t="shared" si="8"/>
         <v>0.45040150292859643</v>
       </c>
+      <c r="AB22">
+        <f t="shared" si="9"/>
+        <v>204.67671405843558</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="10"/>
+        <v>189.88080701806672</v>
+      </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>2643</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>2657</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>130</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2671</v>
-      </c>
-      <c r="P21" s="17"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>2644</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2656</v>
-      </c>
-      <c r="C22">
-        <v>130</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2671</v>
-      </c>
-      <c r="P22" s="17"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>2646</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2647</v>
-      </c>
-      <c r="C23">
-        <v>132</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2655</v>
       </c>
       <c r="E23" t="s">
         <v>2671</v>
       </c>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2658</v>
+        <v>2644</v>
       </c>
       <c r="B24" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
       <c r="C24">
-        <v>133</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2660</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
         <v>2671</v>
       </c>
       <c r="P24" s="17"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2658</v>
+        <v>2646</v>
       </c>
       <c r="B25" t="s">
-        <v>2661</v>
+        <v>2647</v>
       </c>
       <c r="C25">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
         <v>2655</v>
@@ -9927,44 +10115,80 @@
       </c>
       <c r="P25" s="17"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2662</v>
+        <v>2658</v>
       </c>
       <c r="B26" t="s">
-        <v>2663</v>
+        <v>2659</v>
       </c>
       <c r="C26">
         <v>133</v>
       </c>
       <c r="D26" t="s">
-        <v>2655</v>
+        <v>2660</v>
       </c>
       <c r="E26" t="s">
         <v>2671</v>
       </c>
       <c r="P26" s="17"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>2664</v>
+        <v>2658</v>
       </c>
       <c r="B27" t="s">
-        <v>2665</v>
+        <v>2661</v>
       </c>
       <c r="C27">
         <v>133</v>
       </c>
+      <c r="D27" t="s">
+        <v>2655</v>
+      </c>
       <c r="E27" t="s">
         <v>2671</v>
       </c>
       <c r="P27" s="17"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2663</v>
+      </c>
+      <c r="C28">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2655</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2671</v>
+      </c>
+      <c r="P28" s="17"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2665</v>
+      </c>
+      <c r="C29">
+        <v>133</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2671</v>
+      </c>
+      <c r="P29" s="17"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>2707</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E31" t="s">
         <v>2706</v>
       </c>
     </row>

</xml_diff>